<commit_message>
Updated devices and search functionality
</commit_message>
<xml_diff>
--- a/public/docs/Devices.xlsx
+++ b/public/docs/Devices.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="19140" windowHeight="7416"/>
+    <workbookView xWindow="0" yWindow="2436" windowWidth="10992" windowHeight="2376" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Devices" sheetId="2" r:id="rId1"/>
     <sheet name="Devices3(Archive2013-03-26)" sheetId="3" r:id="rId2"/>
     <sheet name="Archive2013-03-26" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A262:K267"/>
 </workbook>
 </file>
 
@@ -4880,7 +4881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W437"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A433" workbookViewId="0">
+    <sheetView topLeftCell="A433" workbookViewId="0">
       <selection activeCell="D438" sqref="D438"/>
     </sheetView>
   </sheetViews>
@@ -43077,7 +43078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S278"/>
   <sheetViews>
-    <sheetView topLeftCell="A262" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
       <selection activeCell="D271" sqref="D271"/>
     </sheetView>
   </sheetViews>

</xml_diff>